<commit_message>
Added: long name to test excel file.
</commit_message>
<xml_diff>
--- a/CertificateGeneratorCoreTests/TestData/example.xlsx
+++ b/CertificateGeneratorCoreTests/TestData/example.xlsx
@@ -43,7 +43,7 @@
     <t xml:space="preserve">English</t>
   </si>
   <si>
-    <t xml:space="preserve">Jane Smith</t>
+    <t xml:space="preserve">Jane Smith en ook nog vele anderen</t>
   </si>
   <si>
     <t xml:space="preserve">2023-06-02</t>
@@ -83,6 +83,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -103,6 +104,7 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -147,8 +149,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -180,92 +186,95 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.67"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="n">
+      <c r="B2" s="2" t="n">
         <v>150</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1" t="n">
+      <c r="B3" s="2" t="n">
         <v>200</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="1" t="n">
+      <c r="B4" s="2" t="n">
         <v>180</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="1" t="n">
+      <c r="B5" s="2" t="n">
         <v>220</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="1" t="n">
+      <c r="B6" s="2" t="n">
         <v>170</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="2" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added: using multiple template files.
</commit_message>
<xml_diff>
--- a/CertificateGeneratorCoreTests/TestData/example.xlsx
+++ b/CertificateGeneratorCoreTests/TestData/example.xlsx
@@ -186,7 +186,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -213,7 +213,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>150</v>
+        <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Changed: date field in BulkTool is now more flexible (string instead of DateOnly).
</commit_message>
<xml_diff>
--- a/CertificateGeneratorCoreTests/TestData/example.xlsx
+++ b/CertificateGeneratorCoreTests/TestData/example.xlsx
@@ -67,7 +67,7 @@
     <t xml:space="preserve">François Dupont</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-06-05</t>
+    <t xml:space="preserve">December 2024</t>
   </si>
 </sst>
 </file>
@@ -186,12 +186,13 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.47"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>